<commit_message>
update insights 2 add Clarifications
</commit_message>
<xml_diff>
--- a/insights/2/contestant_request_stats.xlsx
+++ b/insights/2/contestant_request_stats.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\ioi_project\ioi-grant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\ioi_project\ioi-grant\insights\2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1A3FB9F2-36AF-41B2-B0EF-CD0691864993}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BDC5E9-409D-42AE-8DAB-5BBC511E64B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2019 DAY 1" sheetId="1" r:id="rId1"/>
-    <sheet name="2019 DAY 2" sheetId="2" r:id="rId2"/>
+    <sheet name="2019 DAY 1" sheetId="3" r:id="rId1"/>
+    <sheet name="2019 DAY 2" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="16">
   <si>
     <t>time_grp</t>
   </si>
@@ -67,11 +67,14 @@
   <si>
     <t>throwtrash</t>
   </si>
+  <si>
+    <t>Clarifications</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -911,16 +914,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C70"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E20608-9A76-41F6-9D6E-71CB8FCB5F71}">
+  <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -939,10 +944,10 @@
         <v>43683.208333333336</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -950,10 +955,10 @@
         <v>43683.208333333336</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -961,10 +966,10 @@
         <v>43683.208333333336</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -972,10 +977,10 @@
         <v>43683.208333333336</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -983,10 +988,10 @@
         <v>43683.208333333336</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -994,10 +999,10 @@
         <v>43683.208333333336</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1005,21 +1010,21 @@
         <v>43683.208333333336</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1">
-        <v>26</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>43683.229166666664</v>
+        <v>43683.208333333336</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1027,10 +1032,10 @@
         <v>43683.229166666664</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1049,10 +1054,10 @@
         <v>43683.229166666664</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1060,10 +1065,10 @@
         <v>43683.229166666664</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1071,10 +1076,10 @@
         <v>43683.229166666664</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C14" s="1">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1082,32 +1087,32 @@
         <v>43683.229166666664</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C15" s="1">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>43683.25</v>
+        <v>43683.229166666664</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>43683.25</v>
+        <v>43683.229166666664</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="1">
-        <v>29</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1115,10 +1120,10 @@
         <v>43683.25</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C18" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1126,10 +1131,10 @@
         <v>43683.25</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C19" s="1">
-        <v>10</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1148,10 +1153,10 @@
         <v>43683.25</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C21" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1167,35 +1172,35 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>43683.270833333336</v>
+        <v>43683.25</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C23" s="1">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>43683.270833333336</v>
+        <v>43683.25</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C24" s="1">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>43683.270833333336</v>
+        <v>43683.25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C25" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1214,10 +1219,10 @@
         <v>43683.270833333336</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1">
         <v>8</v>
-      </c>
-      <c r="C27" s="1">
-        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1225,10 +1230,10 @@
         <v>43683.270833333336</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C28" s="1">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1236,54 +1241,54 @@
         <v>43683.270833333336</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C29" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>43683.291666666664</v>
+        <v>43683.270833333336</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C30" s="1">
-        <v>132</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>43683.291666666664</v>
+        <v>43683.270833333336</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C31" s="1">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>43683.291666666664</v>
+        <v>43683.270833333336</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C32" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>43683.291666666664</v>
+        <v>43683.270833333336</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C33" s="1">
-        <v>17</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1291,10 +1296,10 @@
         <v>43683.291666666664</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C34" s="1">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1302,65 +1307,65 @@
         <v>43683.291666666664</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C35" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>43683.3125</v>
+        <v>43683.291666666664</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C36" s="1">
-        <v>18</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>43683.3125</v>
+        <v>43683.291666666664</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C37" s="1">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>43683.3125</v>
+        <v>43683.291666666664</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C38" s="1">
-        <v>48</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>43683.3125</v>
+        <v>43683.291666666664</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C39" s="1">
-        <v>77</v>
+        <v>132</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>43683.3125</v>
+        <v>43683.291666666664</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C40" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1368,10 +1373,10 @@
         <v>43683.3125</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C41" s="1">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1379,76 +1384,76 @@
         <v>43683.3125</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C42" s="1">
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>43683.333333333336</v>
+        <v>43683.3125</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C43" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>43683.333333333336</v>
+        <v>43683.3125</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C44" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>43683.333333333336</v>
+        <v>43683.3125</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C45" s="1">
-        <v>75</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>43683.333333333336</v>
+        <v>43683.3125</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C46" s="1">
-        <v>6</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>43683.333333333336</v>
+        <v>43683.3125</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C47" s="1">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>43683.333333333336</v>
+        <v>43683.3125</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C48" s="1">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1456,205 +1461,205 @@
         <v>43683.333333333336</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C49" s="1">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>43683.354166666664</v>
+        <v>43683.333333333336</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C50" s="1">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>43683.354166666664</v>
+        <v>43683.333333333336</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C51" s="1">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>43683.354166666664</v>
+        <v>43683.333333333336</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C52" s="1">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>43683.354166666664</v>
+        <v>43683.333333333336</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C53" s="1">
-        <v>92</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>43683.354166666664</v>
+        <v>43683.333333333336</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C54" s="1">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>43683.354166666664</v>
+        <v>43683.333333333336</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C55" s="1">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>43683.354166666664</v>
+        <v>43683.333333333336</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C56" s="1">
-        <v>7</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>43683.375</v>
+        <v>43683.354166666664</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C57" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>43683.375</v>
+        <v>43683.354166666664</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C58" s="1">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>43683.375</v>
+        <v>43683.354166666664</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C59" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>43683.375</v>
+        <v>43683.354166666664</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C60" s="1">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>43683.375</v>
+        <v>43683.354166666664</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C61" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>43683.375</v>
+        <v>43683.354166666664</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C62" s="1">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>43683.375</v>
+        <v>43683.354166666664</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C63" s="1">
-        <v>5</v>
+        <v>92</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>43683.375</v>
+        <v>43683.354166666664</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C64" s="1">
-        <v>62</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>43683.395833333336</v>
+        <v>43683.375</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C65" s="1">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>43683.395833333336</v>
+        <v>43683.375</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C66" s="1">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>43683.395833333336</v>
+        <v>43683.375</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C67" s="1">
         <v>9</v>
@@ -1662,34 +1667,144 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>43683.395833333336</v>
+        <v>43683.375</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C68" s="1">
-        <v>44</v>
+        <v>13</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>43683.395833333336</v>
+        <v>43683.375</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C69" s="1">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
+        <v>43683.375</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>43683.375</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>43683.375</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>43683.375</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C73" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
         <v>43683.395833333336</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B74" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>43683.395833333336</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>43683.395833333336</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C76" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>43683.395833333336</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C77" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>43683.395833333336</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>43683.395833333336</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C79" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>43683.395833333336</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C70" s="1">
+      <c r="C80" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1699,16 +1814,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C78"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA275F2B-09B8-4CCD-839A-2BBAD213D4DF}">
+  <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1727,7 +1843,7 @@
         <v>43685.222222222219</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -1738,10 +1854,10 @@
         <v>43685.222222222219</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1749,10 +1865,10 @@
         <v>43685.222222222219</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1760,10 +1876,10 @@
         <v>43685.222222222219</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1771,10 +1887,10 @@
         <v>43685.222222222219</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1782,10 +1898,10 @@
         <v>43685.222222222219</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1793,10 +1909,10 @@
         <v>43685.222222222219</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1804,10 +1920,10 @@
         <v>43685.222222222219</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1815,21 +1931,21 @@
         <v>43685.222222222219</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>43685.243055555555</v>
+        <v>43685.222222222219</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1">
-        <v>37</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1837,10 +1953,10 @@
         <v>43685.243055555555</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1">
-        <v>14</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1848,10 +1964,10 @@
         <v>43685.243055555555</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1859,10 +1975,10 @@
         <v>43685.243055555555</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1870,10 +1986,10 @@
         <v>43685.243055555555</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" s="1">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1881,32 +1997,32 @@
         <v>43685.243055555555</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>43685.263888888891</v>
+        <v>43685.243055555555</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1">
-        <v>3</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>43685.263888888891</v>
+        <v>43685.243055555555</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C18" s="1">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1925,10 +2041,10 @@
         <v>43685.263888888891</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C20" s="1">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1936,10 +2052,10 @@
         <v>43685.263888888891</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C21" s="1">
-        <v>58</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1958,43 +2074,43 @@
         <v>43685.263888888891</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C23" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>43685.284722222219</v>
+        <v>43685.263888888891</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="1">
-        <v>96</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>43685.284722222219</v>
+        <v>43685.263888888891</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C25" s="1">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>43685.284722222219</v>
+        <v>43685.263888888891</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="1">
         <v>13</v>
-      </c>
-      <c r="C26" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2002,10 +2118,10 @@
         <v>43685.284722222219</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C27" s="1">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2013,10 +2129,10 @@
         <v>43685.284722222219</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C28" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2024,10 +2140,10 @@
         <v>43685.284722222219</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C29" s="1">
-        <v>31</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2035,10 +2151,10 @@
         <v>43685.284722222219</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C30" s="1">
-        <v>5</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2046,54 +2162,54 @@
         <v>43685.284722222219</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C31" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>43685.305555555555</v>
+        <v>43685.284722222219</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C32" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>43685.305555555555</v>
+        <v>43685.284722222219</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C33" s="1">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>43685.305555555555</v>
+        <v>43685.284722222219</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>43685.305555555555</v>
+        <v>43685.284722222219</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C35" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -2101,10 +2217,10 @@
         <v>43685.305555555555</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C36" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -2112,10 +2228,10 @@
         <v>43685.305555555555</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C37" s="1">
-        <v>85</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -2123,65 +2239,65 @@
         <v>43685.305555555555</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C38" s="1">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>43685.326388888891</v>
+        <v>43685.305555555555</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C39" s="1">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>43685.326388888891</v>
+        <v>43685.305555555555</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C40" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>43685.326388888891</v>
+        <v>43685.305555555555</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C41" s="1">
-        <v>35</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>43685.326388888891</v>
+        <v>43685.305555555555</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C42" s="1">
-        <v>1</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>43685.326388888891</v>
+        <v>43685.305555555555</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C43" s="1">
-        <v>86</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2189,10 +2305,10 @@
         <v>43685.326388888891</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C44" s="1">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -2200,10 +2316,10 @@
         <v>43685.326388888891</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C45" s="1">
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -2211,224 +2327,224 @@
         <v>43685.326388888891</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C46" s="1">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>43685.347222222219</v>
+        <v>43685.326388888891</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C47" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>43685.347222222219</v>
+        <v>43685.326388888891</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C48" s="1">
-        <v>81</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>43685.347222222219</v>
+        <v>43685.326388888891</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C49" s="1">
-        <v>24</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>43685.347222222219</v>
+        <v>43685.326388888891</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C50" s="1">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>43685.347222222219</v>
+        <v>43685.326388888891</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C51" s="1">
-        <v>21</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>43685.347222222219</v>
+        <v>43685.326388888891</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C52" s="1">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>43685.368055555555</v>
+        <v>43685.347222222219</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C53" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>43685.368055555555</v>
+        <v>43685.347222222219</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C54" s="1">
-        <v>22</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>43685.368055555555</v>
+        <v>43685.347222222219</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C55" s="1">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>43685.368055555555</v>
+        <v>43685.347222222219</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C56" s="1">
-        <v>83</v>
+        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>43685.368055555555</v>
+        <v>43685.347222222219</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C57" s="1">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>43685.368055555555</v>
+        <v>43685.347222222219</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C58" s="1">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>43685.388888888891</v>
+        <v>43685.347222222219</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C59" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>43685.388888888891</v>
+        <v>43685.368055555555</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C60" s="1">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>43685.388888888891</v>
+        <v>43685.368055555555</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C61" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>43685.388888888891</v>
+        <v>43685.368055555555</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C62" s="1">
-        <v>60</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>43685.388888888891</v>
+        <v>43685.368055555555</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C63" s="1">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>43685.388888888891</v>
+        <v>43685.368055555555</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C64" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>43685.388888888891</v>
+        <v>43685.368055555555</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C65" s="1">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>43685.409722222219</v>
+        <v>43685.368055555555</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>7</v>
@@ -2439,7 +2555,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>43685.409722222219</v>
+        <v>43685.388888888891</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>6</v>
@@ -2450,123 +2566,244 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>43685.409722222219</v>
+        <v>43685.388888888891</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C68" s="1">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>43685.409722222219</v>
+        <v>43685.388888888891</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C69" s="1">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>43685.409722222219</v>
+        <v>43685.388888888891</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C70" s="1">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>43685.409722222219</v>
+        <v>43685.388888888891</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C71" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>43685.409722222219</v>
+        <v>43685.388888888891</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C72" s="1">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>43685.430555555555</v>
+        <v>43685.388888888891</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C73" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>43685.430555555555</v>
+        <v>43685.388888888891</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C74" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>43685.430555555555</v>
+        <v>43685.409722222219</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C75" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>43685.430555555555</v>
+        <v>43685.409722222219</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C76" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>43685.430555555555</v>
+        <v>43685.409722222219</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C77" s="1">
-        <v>4</v>
+        <v>31</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
+        <v>43685.409722222219</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C78" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>43685.409722222219</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C79" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>43685.409722222219</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C80" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>43685.409722222219</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C81" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>43685.409722222219</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
         <v>43685.430555555555</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C78" s="1">
-        <v>5</v>
+      <c r="B83" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>43685.430555555555</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C84" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>43685.430555555555</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C85" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>43685.430555555555</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C86" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>43685.430555555555</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>43685.430555555555</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C88" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>43685.430555555555</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89" s="1">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>